<commit_message>
updates code and documentation for the counting of complete lung health checks only (i.e. excluding partially attended contacts)
</commit_message>
<xml_diff>
--- a/data/reference/TLHC data item dictionary.xlsx
+++ b/data/reference/TLHC data item dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B43EE09-122A-4DE5-B940-BFD6048F61B1}"/>
+  <xr:revisionPtr revIDLastSave="325" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF7EB517-D003-43D8-808E-8D16455C8C3C}"/>
   <bookViews>
-    <workbookView xWindow="8490" yWindow="195" windowWidth="20325" windowHeight="19215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataItems" sheetId="1" r:id="rId1"/>
@@ -552,15 +552,6 @@
     <t>First attended LHC</t>
   </si>
   <si>
-    <t>Filters:
-• Eligible for TLHC programme (F1)
-• Valid ParticipantID (F2)
-• Has a valid date in [LHC_Date]
-• [LHC_Attendance] is IN ('Participant attended LHC', 'Participant attended but did not complete LHC')
-• Has a valid [First_Letter_Date]
-If multiple attended records meet the above criteria then take the earliest dated record.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <i/>
@@ -2751,6 +2742,15 @@
       <t xml:space="preserve">
 Median interval (days) per month of [Cancer_Diagnosis_Date]</t>
     </r>
+  </si>
+  <si>
+    <t>Filters:
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Has a valid date in [LHC_Date]
+• [LHC_Attendance] = 'Participant attended LHC'
+• Has a valid [First_Letter_Date]
+If multiple attended records meet the above criteria then take the earliest dated record.</t>
   </si>
 </sst>
 </file>
@@ -2818,29 +2818,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2851,45 +2845,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2962,6 +2917,45 @@
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2976,25 +2970,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}" name="_DataItems" displayName="_DataItems" ref="A1:C51" totalsRowShown="0" headerRowDxfId="2" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}" name="_DataItems" displayName="_DataItems" ref="A1:C51" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:C51" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50FB29E0-4EBB-45EE-B25B-B919FB4F3968}" name="Data Item ID" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{04CC9A59-6BE8-4522-AD37-9E45CB14E2BB}" name="Data Item" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{A3EEB7CC-4AE5-4CAF-87DE-344F3B07528D}" name="Pseudo-logic" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{50FB29E0-4EBB-45EE-B25B-B919FB4F3968}" name="Data Item ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{04CC9A59-6BE8-4522-AD37-9E45CB14E2BB}" name="Data Item" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{A3EEB7CC-4AE5-4CAF-87DE-344F3B07528D}" name="Pseudo-logic" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D9EBE7D-C8C0-4C1A-B311-D0A494BF2FAD}" name="_Filters" displayName="_Filters" ref="A1:D9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D9EBE7D-C8C0-4C1A-B311-D0A494BF2FAD}" name="_Filters" displayName="_Filters" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D9" xr:uid="{6D9EBE7D-C8C0-4C1A-B311-D0A494BF2FAD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9134AC4E-965C-4B40-A198-02E601E046B4}" name="Filter ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{E992744D-9A74-4DD4-890C-650ED1B7D259}" name="Filter criteria" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4ECC91E1-A8B3-44C3-9FC7-5F6571C133F7}" name="Table" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{45EBE059-6C84-4EEF-8FF7-08F2B8F95F3E}" name="Criteria" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{9134AC4E-965C-4B40-A198-02E601E046B4}" name="Filter ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E992744D-9A74-4DD4-890C-650ED1B7D259}" name="Filter criteria" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{4ECC91E1-A8B3-44C3-9FC7-5F6571C133F7}" name="Table" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{45EBE059-6C84-4EEF-8FF7-08F2B8F95F3E}" name="Criteria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3265,7 +3259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3289,553 +3283,553 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>124</v>
+      <c r="C6" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>125</v>
+      <c r="C7" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>126</v>
+      <c r="C8" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>127</v>
+      <c r="C9" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>128</v>
+      <c r="C10" s="4" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>134</v>
+      <c r="C11" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>139</v>
+      <c r="C12" s="4" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>140</v>
+      <c r="C13" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>141</v>
+      <c r="C14" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>142</v>
+      <c r="C15" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>143</v>
+      <c r="C16" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>144</v>
+      <c r="C17" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>145</v>
+      <c r="C18" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>145</v>
+      <c r="C19" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>145</v>
+      <c r="C20" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>145</v>
+      <c r="C21" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>145</v>
+      <c r="C22" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>151</v>
+      <c r="C23" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>149</v>
+      <c r="C24" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>150</v>
+      <c r="C25" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>152</v>
+      <c r="C26" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>153</v>
+      <c r="C27" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>154</v>
+      <c r="C28" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>155</v>
+      <c r="C29" s="4" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>156</v>
+      <c r="C30" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>157</v>
+      <c r="C31" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>158</v>
+      <c r="C32" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>159</v>
+      <c r="C33" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>160</v>
+      <c r="C34" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>161</v>
+      <c r="C35" s="4" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>162</v>
+      <c r="C36" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>164</v>
+      <c r="C37" s="4" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>163</v>
+      <c r="C38" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>165</v>
+      <c r="C39" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>171</v>
+      <c r="C40" s="4" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>170</v>
+      <c r="C41" s="4" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>169</v>
+      <c r="C42" s="4" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>172</v>
+      <c r="C43" s="4" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>173</v>
+      <c r="C44" s="4" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>174</v>
+      <c r="C45" s="4" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>177</v>
+      <c r="C46" s="4" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>176</v>
+      <c r="C47" s="4" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>178</v>
+      <c r="C48" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>74</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>179</v>
+      <c r="C49" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>76</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>180</v>
+      <c r="C50" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>181</v>
+      <c r="C51" s="4" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3851,17 +3845,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB5A504-E72F-4287-8441-1DD37B0D737C}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6"/>
-    <col min="4" max="4" width="93.140625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="10.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="5"/>
+    <col min="4" max="4" width="93.140625" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3889,7 +3883,7 @@
         <v>86</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3928,64 +3922,64 @@
         <v>122</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>123</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>167</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates data item dictionary to match changed dq filters for incidental findings
</commit_message>
<xml_diff>
--- a/data/reference/TLHC data item dictionary.xlsx
+++ b/data/reference/TLHC data item dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="325" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF7EB517-D003-43D8-808E-8D16455C8C3C}"/>
+  <xr:revisionPtr revIDLastSave="327" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07C85FDB-D6CA-4C20-AA33-68FF0374B43B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="375" yWindow="6105" windowWidth="32265" windowHeight="17235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataItems" sheetId="1" r:id="rId1"/>
@@ -1204,11 +1204,1517 @@
     <t>Other incidental finding</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'consolidation'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'tuberculosis'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Records matching ANY 7a-7u are consolidated to a single table.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'mediastinal mass'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'coronary calcification'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'aortic valve calcification'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'thoracic aortic aneurysm'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'pleural effusions/thickening'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'suspicious breast lesion'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'thyroid lesion'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'liver or splenic lesions'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'renal lesions'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'adrenal lesions'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'abdominal aortic aneurysm'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'osteoporosis'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'bone abnormalities'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'fractures with no trauma history'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>Pulmonary incidental finding</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Pulmonary incidental findings (F8)
+• Matched with either 'interstitial lung abnormalities (ilas)' OR 'ila'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Pulmonary incidental findings (F8)
+• Matched with 'respiratory bronchiolitis'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Pulmonary incidental findings (F8)
+• Matched with 'bronchiectasis'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Other incidental findings (F7)
+• Matched with 'other cancers'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Has a valid date in [LDCT_Date]
+• Risk score (F5) is high
+• [LDCT_Outcome] = 'LDCT performed'
+• [Emphysema_Extent] is IN ('Moderate', 'Severe')
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Has a valid date in [Date_offered_smoking_cessation]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [Date_offered_smoking_cessation]</t>
+    </r>
+  </si>
+  <si>
+    <t>Invite_Outcome is NOT in (
+'Participant does not meet age criteria',
+'Participant does not meet smoking criteria',
+'Participant removed from GP list'
+)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Has a valid date in [Date_offered_smoking_cessation]
+• Has a valid date in [Date_started_smoking_cessation]
+• Has a valid date in [Date_ended_smoking_cessation]
+• [Smoking_Cessation_completed_Successfully] = 'Y'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [calc_date_ended_smoking_cessation_yearmon]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Has a valid date in [Date_offered_smoking_cessation]
+• Has a valid date in [Date_started_smoking_cessation]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [calc_date_started_smoking_cessation_yearmon]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Has a valid date in [First_Letter_Date]
+• Earliest attended LHC appointment (F4)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Interval (days) is calculated as: [LHC_Date] - [First_Letter_Date]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Median interval (days) per month of [LHC_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Has a valid date in [First_Letter_Date]
+• LDCT scans (F6)
+• Scans category limited to Initial scans
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Interval (days) is calculated as: [LDCT_Date] - [First_Letter_Date]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Median interval (days) per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Earliest attended LHC appointment (F4)
+• LDCT scans (F6)
+• Scans category limited to Initial scans
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Interval (days) is calculated as: [LDCT_Date] - [LHC_Date]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Median interval (days) per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Has a valid date in [First_Letter_Date]
+• Has a valid date in [Cancer_Diagnosis_Date]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Interval (days) is calculated as: [Cancer_Diagnosis_Date] - [First_Letter_Date]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Median interval (days) per month of [Cancer_Diagnosis_Date]</t>
+    </r>
+  </si>
+  <si>
+    <t>Filters:
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Has a valid date in [LHC_Date]
+• [LHC_Attendance] = 'Participant attended LHC'
+• Has a valid [First_Letter_Date]
+If multiple attended records meet the above criteria then take the earliest dated record.</t>
+  </si>
+  <si>
     <t>Filters:
 • Eligible for TLHC programme (F1)
 • Valid ParticipantID (F2)
 • Has a valid date in [LDCT_Date]
-• High risk score (F5)
 • [LDCT_Outcome] = 'LDCT performed'
 • [Other_Incidental_Findings] is NOT NULL
 The string in [Other_Incidental_Findings] is split into separate findings and each is fuzzy matched to one of the following:
@@ -1232,813 +2738,10 @@
       'other cancers'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'consolidation'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'tuberculosis'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Records matching ANY 7a-7u are consolidated to a single table.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'mediastinal mass'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'coronary calcification'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'aortic valve calcification'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'thoracic aortic aneurysm'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'pleural effusions/thickening'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'suspicious breast lesion'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'thyroid lesion'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'liver or splenic lesions'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'renal lesions'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'adrenal lesions'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'abdominal aortic aneurysm'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'osteoporosis'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'bone abnormalities'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'fractures with no trauma history'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <t>F8</t>
-  </si>
-  <si>
-    <t>Pulmonary incidental finding</t>
-  </si>
-  <si>
     <t>Filters:
 • Eligible for TLHC programme (F1)
 • Valid ParticipantID (F2)
 • Has a valid date in [LDCT_Date]
-• High risk score (F5)
 • [LDCT_Outcome] = 'LDCT performed'
 • [Pulmonary_Incidental_Findings] is NOT NULL
 The string in [Pulmonary_Incidental_Findings] is split into separate findings and each is fuzzy matched to one of the following:
@@ -2046,711 +2749,6 @@
       'respiratory bronchiolitis',
       'interstitial lung abnormalities (ilas)',
       'ila'</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Pulmonary incidental findings (F8)
-• Matched with either 'interstitial lung abnormalities (ilas)' OR 'ila'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Pulmonary incidental findings (F8)
-• Matched with 'respiratory bronchiolitis'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Pulmonary incidental findings (F8)
-• Matched with 'bronchiectasis'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Other incidental findings (F7)
-• Matched with 'other cancers'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Eligible for TLHC programme (F1)
-• Valid ParticipantID (F2)
-• Has a valid date in [LDCT_Date]
-• Risk score (F5) is high
-• [LDCT_Outcome] = 'LDCT performed'
-• [Emphysema_Extent] is IN ('Moderate', 'Severe')
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Eligible for TLHC programme (F1)
-• Valid ParticipantID (F2)
-• Has a valid date in [Date_offered_smoking_cessation]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [Date_offered_smoking_cessation]</t>
-    </r>
-  </si>
-  <si>
-    <t>Invite_Outcome is NOT in (
-'Participant does not meet age criteria',
-'Participant does not meet smoking criteria',
-'Participant removed from GP list'
-)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Eligible for TLHC programme (F1)
-• Valid ParticipantID (F2)
-• Has a valid date in [Date_offered_smoking_cessation]
-• Has a valid date in [Date_started_smoking_cessation]
-• Has a valid date in [Date_ended_smoking_cessation]
-• [Smoking_Cessation_completed_Successfully] = 'Y'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [calc_date_ended_smoking_cessation_yearmon]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Eligible for TLHC programme (F1)
-• Valid ParticipantID (F2)
-• Has a valid date in [Date_offered_smoking_cessation]
-• Has a valid date in [Date_started_smoking_cessation]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [calc_date_started_smoking_cessation_yearmon]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Eligible for TLHC programme (F1)
-• Valid ParticipantID (F2)
-• Has a valid date in [First_Letter_Date]
-• Earliest attended LHC appointment (F4)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Calculation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Interval (days) is calculated as: [LHC_Date] - [First_Letter_Date]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Median interval (days) per month of [LHC_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Eligible for TLHC programme (F1)
-• Valid ParticipantID (F2)
-• Has a valid date in [First_Letter_Date]
-• LDCT scans (F6)
-• Scans category limited to Initial scans
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Calculation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Interval (days) is calculated as: [LDCT_Date] - [First_Letter_Date]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Median interval (days) per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Eligible for TLHC programme (F1)
-• Valid ParticipantID (F2)
-• Earliest attended LHC appointment (F4)
-• LDCT scans (F6)
-• Scans category limited to Initial scans
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Calculation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Interval (days) is calculated as: [LDCT_Date] - [LHC_Date]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Median interval (days) per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Eligible for TLHC programme (F1)
-• Valid ParticipantID (F2)
-• Has a valid date in [First_Letter_Date]
-• Has a valid date in [Cancer_Diagnosis_Date]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Calculation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Interval (days) is calculated as: [Cancer_Diagnosis_Date] - [First_Letter_Date]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Median interval (days) per month of [Cancer_Diagnosis_Date]</t>
-    </r>
-  </si>
-  <si>
-    <t>Filters:
-• Eligible for TLHC programme (F1)
-• Valid ParticipantID (F2)
-• Has a valid date in [LHC_Date]
-• [LHC_Attendance] = 'Participant attended LHC'
-• Has a valid [First_Letter_Date]
-If multiple attended records meet the above criteria then take the earliest dated record.</t>
   </si>
 </sst>
 </file>
@@ -3259,7 +3257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3521,7 +3519,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3532,7 +3530,7 @@
         <v>94</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3543,7 +3541,7 @@
         <v>95</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3554,7 +3552,7 @@
         <v>96</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3565,7 +3563,7 @@
         <v>97</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3576,7 +3574,7 @@
         <v>98</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3587,7 +3585,7 @@
         <v>99</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3598,7 +3596,7 @@
         <v>100</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3609,7 +3607,7 @@
         <v>101</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3620,7 +3618,7 @@
         <v>102</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3631,7 +3629,7 @@
         <v>103</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3642,7 +3640,7 @@
         <v>104</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3653,7 +3651,7 @@
         <v>105</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3664,7 +3662,7 @@
         <v>106</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3675,7 +3673,7 @@
         <v>107</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3686,7 +3684,7 @@
         <v>108</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3697,7 +3695,7 @@
         <v>109</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3708,7 +3706,7 @@
         <v>110</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3719,7 +3717,7 @@
         <v>111</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3730,7 +3728,7 @@
         <v>112</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3741,7 +3739,7 @@
         <v>113</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="150" x14ac:dyDescent="0.25">
@@ -3752,7 +3750,7 @@
         <v>114</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -3763,7 +3761,7 @@
         <v>67</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="120" x14ac:dyDescent="0.25">
@@ -3774,7 +3772,7 @@
         <v>69</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="150" x14ac:dyDescent="0.25">
@@ -3785,7 +3783,7 @@
         <v>71</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -3796,7 +3794,7 @@
         <v>73</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="180" x14ac:dyDescent="0.25">
@@ -3807,7 +3805,7 @@
         <v>75</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="180" x14ac:dyDescent="0.25">
@@ -3818,7 +3816,7 @@
         <v>77</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -3829,7 +3827,7 @@
         <v>79</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3845,8 +3843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB5A504-E72F-4287-8441-1DD37B0D737C}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3883,7 +3881,7 @@
         <v>86</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3925,7 +3923,7 @@
         <v>131</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3956,7 +3954,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="405" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>145</v>
       </c>
@@ -3967,19 +3965,19 @@
         <v>135</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates definitions for metrics 5d-5g, adds definition for metric 5h and adds change column to clarify what has changed.
</commit_message>
<xml_diff>
--- a/data/reference/TLHC data item dictionary.xlsx
+++ b/data/reference/TLHC data item dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="327" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07C85FDB-D6CA-4C20-AA33-68FF0374B43B}"/>
+  <xr:revisionPtr revIDLastSave="364" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EB84248-D048-4C2A-9717-1B15E1B20CC1}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="6105" windowWidth="32265" windowHeight="17235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="3450" windowWidth="25365" windowHeight="17235" xr2:uid="{154B46B6-DB68-4069-9312-B75F16A26CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="DataItems" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="190">
   <si>
     <t>Data Item</t>
   </si>
@@ -117,25 +117,13 @@
     <t>5d</t>
   </si>
   <si>
-    <t>3 month follow up LDCT scan performed</t>
-  </si>
-  <si>
     <t>5e</t>
   </si>
   <si>
-    <t>12 month follow up LDCT scan performed</t>
-  </si>
-  <si>
     <t>5f</t>
   </si>
   <si>
-    <t>24 month follow up LDCT scan performed</t>
-  </si>
-  <si>
     <t>5g</t>
-  </si>
-  <si>
-    <t>48 month surveillance LDCT scan performed</t>
   </si>
   <si>
     <t>6a</t>
@@ -1071,104 +1059,6 @@
 • Scans (F6)
 • [LDCT_Outcome] = 'LDCT performed'
 • Interval from initial scan between 335 to 465 days
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Scans (F6)
-• [LDCT_Outcome] = 'LDCT performed'
-• Interval from initial scan between 669 to 850 days
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aggregation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Filters:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Scans (F6)
-• [LDCT_Outcome] = 'LDCT performed'
-• Interval from initial scan between 1005 to 1275 days
 </t>
     </r>
     <r>
@@ -2749,6 +2639,188 @@
       'respiratory bronchiolitis',
       'interstitial lung abnormalities (ilas)',
       'ila'</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>3 month follow up nodule surveillance LDCT scan performed</t>
+  </si>
+  <si>
+    <t>05/10/2023 - Added 'nodule surveillance' to reflect current description</t>
+  </si>
+  <si>
+    <t>12 month follow up nodule surveillance LDCT scan performed</t>
+  </si>
+  <si>
+    <t>24 month incident screening round LDCT scan performed</t>
+  </si>
+  <si>
+    <t>48 month incident screening round LDCT scan performed</t>
+  </si>
+  <si>
+    <t>05/10/2023 - Added 'incident screening round' to reflect current description
+05/10/2023 - Reduced upper days limit from 850 to 791 to avoid overlap with metric 5h</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Scans (F6)
+• [LDCT_Outcome] = 'LDCT performed'
+• Interval from initial scan between 669 to 791 days
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <t>05/10/2023 - Added 'incident screening round' to reflect current description
+05/10/2023 - Corrected interval to reflect the 48-month scan</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Scans (F6)
+• [LDCT_Outcome] = 'LDCT performed'
+• Interval from initial scan between 1400 to 1521 days
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>Nodule surveillance LDCT scan performed from a 24 months incident screening round scan onward</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Scans (F6)
+• [LDCT_Outcome] = 'LDCT performed'
+• Interval from initial scan between 792 to 1399 days OR above 1521 days
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [LDCT_Date]</t>
+    </r>
+  </si>
+  <si>
+    <t>05/10/2023 - New metric</t>
   </si>
 </sst>
 </file>
@@ -2816,7 +2888,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2837,12 +2909,39 @@
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2968,25 +3067,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}" name="_DataItems" displayName="_DataItems" ref="A1:C51" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:C51" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50FB29E0-4EBB-45EE-B25B-B919FB4F3968}" name="Data Item ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{04CC9A59-6BE8-4522-AD37-9E45CB14E2BB}" name="Data Item" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{A3EEB7CC-4AE5-4CAF-87DE-344F3B07528D}" name="Pseudo-logic" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}" name="_DataItems" displayName="_DataItems" ref="A1:D52" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:D52" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{50FB29E0-4EBB-45EE-B25B-B919FB4F3968}" name="Data Item ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{04CC9A59-6BE8-4522-AD37-9E45CB14E2BB}" name="Data Item" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{A3EEB7CC-4AE5-4CAF-87DE-344F3B07528D}" name="Pseudo-logic" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{0D658BA4-4833-4589-B32E-E28F28CBDBBF}" name="Change" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D9EBE7D-C8C0-4C1A-B311-D0A494BF2FAD}" name="_Filters" displayName="_Filters" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D9" xr:uid="{6D9EBE7D-C8C0-4C1A-B311-D0A494BF2FAD}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9134AC4E-965C-4B40-A198-02E601E046B4}" name="Filter ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{E992744D-9A74-4DD4-890C-650ED1B7D259}" name="Filter criteria" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{4ECC91E1-A8B3-44C3-9FC7-5F6571C133F7}" name="Table" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{45EBE059-6C84-4EEF-8FF7-08F2B8F95F3E}" name="Criteria" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D9EBE7D-C8C0-4C1A-B311-D0A494BF2FAD}" name="_Filters" displayName="_Filters" ref="A1:E9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:E9" xr:uid="{6D9EBE7D-C8C0-4C1A-B311-D0A494BF2FAD}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{9134AC4E-965C-4B40-A198-02E601E046B4}" name="Filter ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{E992744D-9A74-4DD4-890C-650ED1B7D259}" name="Filter criteria" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{4ECC91E1-A8B3-44C3-9FC7-5F6571C133F7}" name="Table" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{45EBE059-6C84-4EEF-8FF7-08F2B8F95F3E}" name="Criteria" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{8646C252-4D32-41D4-866E-A7F7EAC80526}" name="Change" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3255,32 +3356,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="3" customWidth="1"/>
     <col min="2" max="2" width="57" style="3" customWidth="1"/>
     <col min="3" max="3" width="93.7109375" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="44.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -3288,10 +3391,11 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -3299,10 +3403,11 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -3310,10 +3415,11 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -3321,10 +3427,11 @@
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
@@ -3332,10 +3439,11 @@
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
@@ -3343,10 +3451,11 @@
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -3354,10 +3463,11 @@
         <v>14</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
@@ -3365,10 +3475,11 @@
         <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
@@ -3376,10 +3487,11 @@
         <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
@@ -3387,10 +3499,11 @@
         <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -3398,10 +3511,11 @@
         <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
@@ -3409,426 +3523,487 @@
         <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="B15" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="B17" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="B28" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C41" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C45" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="4" t="s">
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>178</v>
-      </c>
+      <c r="C52" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3841,11 +4016,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB5A504-E72F-4287-8441-1DD37B0D737C}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3853,132 +4026,146 @@
     <col min="2" max="2" width="39.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="5"/>
     <col min="4" max="4" width="93.140625" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="5"/>
+    <col min="5" max="5" width="44.7109375" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="C5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="405" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>159</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>181</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="E9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds metric 14 to the dictionary
</commit_message>
<xml_diff>
--- a/data/reference/TLHC data item dictionary.xlsx
+++ b/data/reference/TLHC data item dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="364" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EB84248-D048-4C2A-9717-1B15E1B20CC1}"/>
+  <xr:revisionPtr revIDLastSave="372" documentId="11_F25DC773A252ABDACC10485B515949AE5BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D48D422-601F-49AF-B008-1A57474D2646}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="3450" windowWidth="25365" windowHeight="17235" xr2:uid="{154B46B6-DB68-4069-9312-B75F16A26CB3}"/>
+    <workbookView xWindow="2880" yWindow="645" windowWidth="23610" windowHeight="17235" xr2:uid="{154B46B6-DB68-4069-9312-B75F16A26CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="DataItems" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="192">
   <si>
     <t>Data Item</t>
   </si>
@@ -2821,6 +2821,61 @@
   </si>
   <si>
     <t>05/10/2023 - New metric</t>
+  </si>
+  <si>
+    <t>Referred to Lung Cancer Pathway following LDCT scan</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Filters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Eligible for TLHC programme (F1)
+• Valid ParticipantID (F2)
+• Has a valid date in [LDCT_Date]
+• Has a valid date in [Date_Referral_Lung_Cancer] in the LDCT table
+• Risk score (F5) is high
+• [LDCT_Outcome] = 'LDCT performed'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aggregation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Count of DISTINCT ParticipantID per month of [Date_Referral_Lung_Cancer]</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2888,7 +2943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2910,13 +2965,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3067,26 +3119,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}" name="_DataItems" displayName="_DataItems" ref="A1:D52" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:D52" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}" name="_DataItems" displayName="_DataItems" ref="A1:D53" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:D53" xr:uid="{3790E45B-F5D7-446C-A4D2-9687BFBEE486}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{50FB29E0-4EBB-45EE-B25B-B919FB4F3968}" name="Data Item ID" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{04CC9A59-6BE8-4522-AD37-9E45CB14E2BB}" name="Data Item" dataDxfId="9"/>
     <tableColumn id="4" xr3:uid="{A3EEB7CC-4AE5-4CAF-87DE-344F3B07528D}" name="Pseudo-logic" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{0D658BA4-4833-4589-B32E-E28F28CBDBBF}" name="Change" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{0D658BA4-4833-4589-B32E-E28F28CBDBBF}" name="Change" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D9EBE7D-C8C0-4C1A-B311-D0A494BF2FAD}" name="_Filters" displayName="_Filters" ref="A1:E9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D9EBE7D-C8C0-4C1A-B311-D0A494BF2FAD}" name="_Filters" displayName="_Filters" ref="A1:E9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E9" xr:uid="{6D9EBE7D-C8C0-4C1A-B311-D0A494BF2FAD}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9134AC4E-965C-4B40-A198-02E601E046B4}" name="Filter ID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{E992744D-9A74-4DD4-890C-650ED1B7D259}" name="Filter criteria" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{4ECC91E1-A8B3-44C3-9FC7-5F6571C133F7}" name="Table" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{45EBE059-6C84-4EEF-8FF7-08F2B8F95F3E}" name="Criteria" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9134AC4E-965C-4B40-A198-02E601E046B4}" name="Filter ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{E992744D-9A74-4DD4-890C-650ED1B7D259}" name="Filter criteria" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{4ECC91E1-A8B3-44C3-9FC7-5F6571C133F7}" name="Table" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{45EBE059-6C84-4EEF-8FF7-08F2B8F95F3E}" name="Criteria" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{8646C252-4D32-41D4-866E-A7F7EAC80526}" name="Change" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3356,9 +3408,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3379,7 +3433,7 @@
       <c r="C1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3393,7 +3447,7 @@
       <c r="C2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -3405,7 +3459,7 @@
       <c r="C3" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -3417,7 +3471,7 @@
       <c r="C4" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -3429,7 +3483,7 @@
       <c r="C5" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -3441,7 +3495,7 @@
       <c r="C6" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -3453,7 +3507,7 @@
       <c r="C7" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -3465,7 +3519,7 @@
       <c r="C8" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -3477,7 +3531,7 @@
       <c r="C9" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -3489,7 +3543,7 @@
       <c r="C10" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -3501,7 +3555,7 @@
       <c r="C11" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -3513,7 +3567,7 @@
       <c r="C12" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -3525,7 +3579,7 @@
       <c r="C13" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -3537,7 +3591,7 @@
       <c r="C14" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="4" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3551,7 +3605,7 @@
       <c r="C15" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="4" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3565,7 +3619,7 @@
       <c r="C16" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="4" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3579,21 +3633,21 @@
       <c r="C17" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="4" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="4" t="s">
         <v>187</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="4" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3607,7 +3661,7 @@
       <c r="C19" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
@@ -3619,7 +3673,7 @@
       <c r="C20" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="8"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
@@ -3631,7 +3685,7 @@
       <c r="C21" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="8"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -3643,7 +3697,7 @@
       <c r="C22" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D22" s="8"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -3655,7 +3709,7 @@
       <c r="C23" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="8"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
@@ -3667,7 +3721,7 @@
       <c r="C24" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D24" s="8"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -3679,7 +3733,7 @@
       <c r="C25" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
@@ -3691,7 +3745,7 @@
       <c r="C26" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -3703,7 +3757,7 @@
       <c r="C27" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D27" s="8"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -3715,7 +3769,7 @@
       <c r="C28" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="8"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -3727,7 +3781,7 @@
       <c r="C29" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D29" s="8"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -3739,7 +3793,7 @@
       <c r="C30" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D30" s="8"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
@@ -3751,7 +3805,7 @@
       <c r="C31" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D31" s="8"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -3763,7 +3817,7 @@
       <c r="C32" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D32" s="8"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
@@ -3775,7 +3829,7 @@
       <c r="C33" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="8"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
@@ -3787,7 +3841,7 @@
       <c r="C34" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D34" s="8"/>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
@@ -3799,7 +3853,7 @@
       <c r="C35" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D35" s="8"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -3811,7 +3865,7 @@
       <c r="C36" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="8"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
@@ -3823,7 +3877,7 @@
       <c r="C37" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D37" s="8"/>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
@@ -3835,7 +3889,7 @@
       <c r="C38" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D38" s="8"/>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
@@ -3847,7 +3901,7 @@
       <c r="C39" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D39" s="8"/>
+      <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
@@ -3859,7 +3913,7 @@
       <c r="C40" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D40" s="8"/>
+      <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
@@ -3871,7 +3925,7 @@
       <c r="C41" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D41" s="8"/>
+      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
@@ -3883,7 +3937,7 @@
       <c r="C42" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D42" s="8"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
@@ -3895,7 +3949,7 @@
       <c r="C43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="8"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
@@ -3907,7 +3961,7 @@
       <c r="C44" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D44" s="8"/>
+      <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
@@ -3919,7 +3973,7 @@
       <c r="C45" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D45" s="8"/>
+      <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -3931,7 +3985,7 @@
       <c r="C46" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D46" s="8"/>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
@@ -3943,7 +3997,7 @@
       <c r="C47" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D47" s="8"/>
+      <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
@@ -3955,7 +4009,7 @@
       <c r="C48" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D48" s="8"/>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
@@ -3967,7 +4021,7 @@
       <c r="C49" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D49" s="8"/>
+      <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
@@ -3979,7 +4033,7 @@
       <c r="C50" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D50" s="8"/>
+      <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
@@ -3991,7 +4045,7 @@
       <c r="C51" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D51" s="8"/>
+      <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
@@ -4003,7 +4057,19 @@
       <c r="C52" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D52" s="8"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
+        <v>14</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D53" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4043,7 +4109,7 @@
       <c r="D1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="4" t="s">
         <v>176</v>
       </c>
     </row>
@@ -4060,7 +4126,7 @@
       <c r="D2" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -4075,7 +4141,7 @@
       <c r="D3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -4090,7 +4156,7 @@
       <c r="D4" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -4105,7 +4171,7 @@
       <c r="D5" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -4120,7 +4186,7 @@
       <c r="D6" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -4135,7 +4201,7 @@
       <c r="D7" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -4150,7 +4216,7 @@
       <c r="D8" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -4165,7 +4231,7 @@
       <c r="D9" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>